<commit_message>
Devices Script Added and Configuration Changes added
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\TruckX\ExcelInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B46464E-51DE-4A05-A265-6B7B5A94C316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805CB65B-F4F2-43D2-A886-17105748D0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Truck" sheetId="1" r:id="rId1"/>
+    <sheet name="Trailer" sheetId="2" r:id="rId2"/>
+    <sheet name="Device" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="4" r:id="rId4"/>
+    <sheet name="Configuration" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,36 +29,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+  <si>
+    <t>Auto Generated</t>
+  </si>
+  <si>
+    <t>VIN Number</t>
+  </si>
+  <si>
+    <t>Truck Identifier</t>
+  </si>
+  <si>
+    <t>Registration No</t>
+  </si>
+  <si>
+    <t>MH12AB1010</t>
+  </si>
+  <si>
+    <t>Insurance Name</t>
+  </si>
+  <si>
+    <t>Insurance Number</t>
+  </si>
+  <si>
+    <t>Cargo Insurance Name</t>
+  </si>
+  <si>
+    <t>Cargo Insurance Number</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>Cargo Name</t>
+  </si>
+  <si>
+    <t>Cargo Number</t>
+  </si>
+  <si>
+    <t>Trailer Identifier</t>
+  </si>
+  <si>
+    <t>Assign Truck</t>
+  </si>
+  <si>
+    <t>Pick up from Truck Tab</t>
+  </si>
+  <si>
+    <t>Device Name</t>
+  </si>
+  <si>
+    <t>Device Id</t>
+  </si>
+  <si>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>User Name</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Abhijeet</t>
-  </si>
-  <si>
-    <t>Nagarkar123</t>
-  </si>
-  <si>
-    <t>Abhi</t>
-  </si>
-  <si>
-    <t>Abhijeet123</t>
-  </si>
-  <si>
-    <t>Nagarkar</t>
-  </si>
-  <si>
-    <t>Nagarkar1234</t>
-  </si>
-  <si>
-    <t>AbhiNagarkar</t>
-  </si>
-  <si>
-    <t>Abhi123</t>
+    <t>demo@truckx.com</t>
+  </si>
+  <si>
+    <t>Abcd1234</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Send Mail</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>https://web.truckx.com/#/login</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>Cloud Dashcam</t>
   </si>
 </sst>
 </file>
@@ -66,7 +132,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -91,8 +157,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,52 +440,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B27B28-C858-42C1-AF0A-315CAD5F91AA}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFF580C-C183-4F41-A812-FC05BC81DA7C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -426,14 +593,81 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B27B28-C858-42C1-AF0A-315CAD5F91AA}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBCFDD8-0AF2-4839-877C-8370929A88EB}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A180C9-7F15-49B0-B3D4-02FC6D435996}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Script to caught exception and show in Extend Report
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805CB65B-F4F2-43D2-A886-17105748D0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A496ED61-1A0B-4029-8582-16E4FA50BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B27B28-C858-42C1-AF0A-315CAD5F91AA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
   <cols>
@@ -555,7 +555,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A180C9-7F15-49B0-B3D4-02FC6D435996}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>

</xml_diff>

<commit_message>
Assets and Tracking Script added
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A496ED61-1A0B-4029-8582-16E4FA50BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46487A26-CFEC-4AAF-B032-324D17407D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Device" sheetId="3" r:id="rId3"/>
     <sheet name="Login" sheetId="4" r:id="rId4"/>
     <sheet name="Configuration" sheetId="5" r:id="rId5"/>
+    <sheet name="Company_Profile" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Auto Generated</t>
   </si>
@@ -106,9 +107,6 @@
     <t>Send Mail</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>https://web.truckx.com/#/login</t>
   </si>
   <si>
@@ -122,6 +120,21 @@
   </si>
   <si>
     <t>Cloud Dashcam</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DOT</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Zeus Transport Inc. 3</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -519,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B27B28-C858-42C1-AF0A-315CAD5F91AA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
   <cols>
@@ -569,7 +582,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.7">
@@ -585,7 +598,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -648,15 +661,15 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.7">
@@ -664,10 +677,54 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB39652-3F9D-478D-87AC-DC06E4A16354}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123412346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted Drivers Script added
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46487A26-CFEC-4AAF-B032-324D17407D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBEC782-CC9E-45AF-B200-1ED2A8196422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
     <t>Zeus Transport Inc. 3</t>
   </si>
   <si>
-    <t>no</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A180C9-7F15-49B0-B3D4-02FC6D435996}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB39652-3F9D-478D-87AC-DC06E4A16354}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>

</xml_diff>

<commit_message>
AdminRegistration,ForgotPassword and Logout Code added
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A496ED61-1A0B-4029-8582-16E4FA50BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16185" windowHeight="6615" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Truck" sheetId="1" r:id="rId1"/>
@@ -18,8 +12,10 @@
     <sheet name="Device" sheetId="3" r:id="rId3"/>
     <sheet name="Login" sheetId="4" r:id="rId4"/>
     <sheet name="Configuration" sheetId="5" r:id="rId5"/>
+    <sheet name="ForgotPassword" sheetId="6" r:id="rId6"/>
+    <sheet name="AdminRegistration" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Auto Generated</t>
   </si>
@@ -123,16 +119,69 @@
   <si>
     <t>Cloud Dashcam</t>
   </si>
+  <si>
+    <t>adminemail</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>Rupali</t>
+  </si>
+  <si>
+    <t>Jagtap</t>
+  </si>
+  <si>
+    <t>rupali@truckx.com</t>
+  </si>
+  <si>
+    <t>cus_LaajxEVariHxrh</t>
+  </si>
+  <si>
+    <t>CarrierName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TruckX Test Carrier </t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>3301 c sac</t>
+  </si>
+  <si>
+    <t>Central Time (US &amp; Canada)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -154,14 +203,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,28 +484,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -461,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -469,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -477,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -485,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -493,7 +545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -501,7 +553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,19 +568,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B27B28-C858-42C1-AF0A-315CAD5F91AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -536,7 +588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -551,20 +603,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFF580C-C183-4F41-A812-FC05BC81DA7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -572,7 +624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -580,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -594,28 +646,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBCFDD8-0AF2-4839-877C-8370929A88EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -624,26 +676,29 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A180C9-7F15-49B0-B3D4-02FC6D435996}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -651,7 +706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -659,7 +714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -670,4 +725,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Trip History and Utilization Report
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98E3DFE-E19E-4FD4-96FF-78A47452C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA4B982-41DA-4C24-8CF0-354FDF870146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="5" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Trailer" sheetId="2" r:id="rId4"/>
     <sheet name="Device" sheetId="3" r:id="rId5"/>
     <sheet name="Company_Profile" sheetId="8" r:id="rId6"/>
-    <sheet name="ForgotPassword" sheetId="6" r:id="rId7"/>
-    <sheet name="AdminRegistration" sheetId="7" r:id="rId8"/>
+    <sheet name="Drivers" sheetId="9" r:id="rId7"/>
+    <sheet name="ForgotPassword" sheetId="6" r:id="rId8"/>
+    <sheet name="AdminRegistration" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Auto Generated</t>
   </si>
@@ -179,6 +180,33 @@
   </si>
   <si>
     <t>DOT</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Abhijeet</t>
+  </si>
+  <si>
+    <t>Nagarkar</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>truckxdriver@gmail.com</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>800-793-9513</t>
+  </si>
+  <si>
+    <t>b111111111111</t>
   </si>
 </sst>
 </file>
@@ -706,7 +734,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -748,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064BC286-3FB6-49F9-B31D-DF90FBC3FEB0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -787,6 +815,69 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76A533F-F939-41B5-A388-5A206504D8AB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{993A6CAA-3077-43F8-AB71-FD73B366277B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -816,7 +907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Duty Status, Trip History, Utilization Report
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA4B982-41DA-4C24-8CF0-354FDF870146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC680D62-CBCA-4364-8514-154E8841582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="5" r:id="rId1"/>
@@ -819,7 +819,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>

</xml_diff>

<commit_message>
Reports and Driver Page Automation Script Added
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC680D62-CBCA-4364-8514-154E8841582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769D73E-D5E1-4F8E-97C3-F2A6E106A85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,25 +188,25 @@
     <t>Last Name</t>
   </si>
   <si>
+    <t>Nagarkar</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>truckxdriver@gmail.com</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>911-000-000</t>
+  </si>
+  <si>
     <t>Abhijeet</t>
   </si>
   <si>
-    <t>Nagarkar</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>truckxdriver@gmail.com</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>800-793-9513</t>
-  </si>
-  <si>
-    <t>b111111111111</t>
+    <t>AI1111111111</t>
   </si>
 </sst>
 </file>
@@ -251,11 +251,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,26 +785,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>123412346</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -819,7 +818,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -833,7 +832,7 @@
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.7">
@@ -841,15 +840,15 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.7">
@@ -857,12 +856,12 @@
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Pre/Post Trip,Billing Details Script added and reduced execution time
</commit_message>
<xml_diff>
--- a/ExcelInput/input.xlsx
+++ b/ExcelInput/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769D73E-D5E1-4F8E-97C3-F2A6E106A85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4753EA-8D7D-4FA2-9070-DDEE37DEEDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,7 +206,7 @@
     <t>Abhijeet</t>
   </si>
   <si>
-    <t>AI1111111111</t>
+    <t>AQ1111111111</t>
   </si>
 </sst>
 </file>
@@ -818,7 +818,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>

</xml_diff>